<commit_message>
enviando segundo commit com as alterações nos arquivos
</commit_message>
<xml_diff>
--- a/arquivo02.xlsx
+++ b/arquivo02.xlsx
@@ -16,6 +16,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>commit 02</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +77,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +122,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +157,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +339,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="53.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>